<commit_message>
some little fixes added
</commit_message>
<xml_diff>
--- a/uploads/uploadedRoutesDataExcelFile.xlsx
+++ b/uploads/uploadedRoutesDataExcelFile.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="224">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="222">
   <si>
     <t>მარშრუტის №</t>
   </si>
@@ -682,12 +682,6 @@
   </si>
   <si>
     <t>ვაკე - საბურთალო</t>
-  </si>
-  <si>
-    <t>მერაბ  კოსტავას ქ. (#69-ის მიდებარედ) - გიორგი სააკაძის მოედანი - ჟიული შარტავას ქ. - ანა კალანდაძის ქ. - პეკინის გამზირი - ვაჟა ფშაველას გამზირი - მიხეილ თამარაშვილის გამზირი - ილია ჭავჭავაძის გამზირი  - პეტრე მელიქიშვილის ქ. - მერაბ კოსტავას ქ.  (#69-ის მიდებარედ)(წრიული).</t>
-  </si>
-  <si>
-    <t>საბურთალო-ვაკე</t>
   </si>
   <si>
     <t>მ/ს "დიდუბე" (ქვედა გასასვლელი) (ტრანსპორტის ქ. #1-ის მიმდებარედ) - აკაკი წერეთლის გამზირი - შალიკაშვილის ხიდი - გრიგოლ რობაქიძის გამზირი - დავით აღმაშენებლის ხეივანი - ფარნავაზ მეფის გამზირი - ასი ათასი მოწამის ქ. - მუხათგვერდის ქ. (მუხათგვერდის სასაფლაო)
@@ -1260,8 +1254,8 @@
   <dimension ref="A1:D115"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B1" sqref="A1:B1048576"/>
+      <pane ySplit="1" topLeftCell="A107" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A115" sqref="A115:D115"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1293,7 +1287,7 @@
         <v>4</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>5</v>
@@ -1307,7 +1301,7 @@
         <v>6</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>7</v>
@@ -1321,10 +1315,10 @@
         <v>8</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="27.9" customHeight="1">
@@ -1366,7 +1360,7 @@
         <v>7</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="27.9" customHeight="1">
@@ -1618,7 +1612,7 @@
         <v>51</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="27.9" customHeight="1">
@@ -1629,7 +1623,7 @@
         <v>52</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="D26" s="3" t="s">
         <v>53</v>
@@ -1643,7 +1637,7 @@
         <v>54</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="D27" s="3" t="s">
         <v>55</v>
@@ -1657,7 +1651,7 @@
         <v>56</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="D28" s="3" t="s">
         <v>5</v>
@@ -1741,7 +1735,7 @@
         <v>67</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="D34" s="3" t="s">
         <v>34</v>
@@ -1839,7 +1833,7 @@
         <v>82</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="D41" s="3" t="s">
         <v>7</v>
@@ -1856,7 +1850,7 @@
         <v>84</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="27.9" customHeight="1">
@@ -1870,7 +1864,7 @@
         <v>84</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="27.9" customHeight="1">
@@ -1884,7 +1878,7 @@
         <v>84</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="45" spans="1:4" ht="27.9" customHeight="1">
@@ -1895,10 +1889,10 @@
         <v>89</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="46" spans="1:4" ht="27.9" customHeight="1">
@@ -1912,7 +1906,7 @@
         <v>91</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="27.9" customHeight="1">
@@ -1934,7 +1928,7 @@
         <v>50</v>
       </c>
       <c r="B48" s="5" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="C48" s="3" t="s">
         <v>94</v>
@@ -1965,7 +1959,7 @@
         <v>97</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="D50" s="3" t="s">
         <v>7</v>
@@ -1979,7 +1973,7 @@
         <v>98</v>
       </c>
       <c r="C51" s="8" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="D51" s="3" t="s">
         <v>125</v>
@@ -2024,7 +2018,7 @@
         <v>58</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="55" spans="1:4" ht="27.9" customHeight="1">
@@ -2063,7 +2057,7 @@
         <v>106</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="D57" s="3" t="s">
         <v>34</v>
@@ -2080,7 +2074,7 @@
         <v>108</v>
       </c>
       <c r="D58" s="3" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="59" spans="1:4" ht="27.9" customHeight="1">
@@ -2091,7 +2085,7 @@
         <v>109</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="D59" s="3" t="s">
         <v>110</v>
@@ -2105,7 +2099,7 @@
         <v>111</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="D60" s="3" t="s">
         <v>125</v>
@@ -2119,10 +2113,10 @@
         <v>112</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="D61" s="3" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="62" spans="1:4" ht="27.9" customHeight="1">
@@ -2133,7 +2127,7 @@
         <v>113</v>
       </c>
       <c r="C62" s="3" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="D62" s="3" t="s">
         <v>125</v>
@@ -2144,13 +2138,13 @@
         <v>69</v>
       </c>
       <c r="B63" s="5" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="C63" s="3" t="s">
         <v>17</v>
       </c>
       <c r="D63" s="6" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="64" spans="1:4" ht="27.9" customHeight="1">
@@ -2161,7 +2155,7 @@
         <v>114</v>
       </c>
       <c r="C64" s="3" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="D64" s="3" t="s">
         <v>34</v>
@@ -2189,7 +2183,7 @@
         <v>116</v>
       </c>
       <c r="C66" s="3" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="D66" s="3" t="s">
         <v>117</v>
@@ -2206,7 +2200,7 @@
         <v>96</v>
       </c>
       <c r="D67" s="3" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="68" spans="1:4" ht="27.9" customHeight="1">
@@ -2276,7 +2270,7 @@
         <v>129</v>
       </c>
       <c r="D72" s="3" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="73" spans="1:4" ht="27.9" customHeight="1">
@@ -2413,10 +2407,10 @@
         <v>146</v>
       </c>
       <c r="C82" s="3" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="D82" s="3" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="83" spans="1:4" ht="27.9" customHeight="1">
@@ -2444,7 +2438,7 @@
         <v>108</v>
       </c>
       <c r="D84" s="7" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="85" spans="1:4" ht="27.9" customHeight="1">
@@ -2570,7 +2564,7 @@
         <v>164</v>
       </c>
       <c r="D93" s="3" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="94" spans="1:4" ht="27.9" customHeight="1">
@@ -2637,7 +2631,7 @@
         <v>171</v>
       </c>
       <c r="C98" s="3" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="D98" s="3" t="s">
         <v>125</v>
@@ -2651,7 +2645,7 @@
         <v>172</v>
       </c>
       <c r="C99" s="3" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="D99" s="3" t="s">
         <v>173</v>
@@ -2690,13 +2684,13 @@
         <v>169</v>
       </c>
       <c r="B102" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="C102" s="7" t="s">
+        <v>195</v>
+      </c>
+      <c r="D102" s="7" t="s">
         <v>196</v>
-      </c>
-      <c r="C102" s="7" t="s">
-        <v>197</v>
-      </c>
-      <c r="D102" s="7" t="s">
-        <v>198</v>
       </c>
     </row>
     <row r="103" spans="1:4" ht="27.9" customHeight="1">
@@ -2710,7 +2704,7 @@
         <v>117</v>
       </c>
       <c r="D103" s="3" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="104" spans="1:4" ht="27.9" customHeight="1">
@@ -2868,18 +2862,10 @@
       </c>
     </row>
     <row r="115" spans="1:4" ht="27.9" customHeight="1">
-      <c r="A115" s="1">
-        <v>387</v>
-      </c>
-      <c r="B115" s="4" t="s">
-        <v>192</v>
-      </c>
-      <c r="C115" s="3" t="s">
-        <v>193</v>
-      </c>
-      <c r="D115" s="3" t="s">
-        <v>72</v>
-      </c>
+      <c r="A115" s="1"/>
+      <c r="B115" s="4"/>
+      <c r="C115" s="3"/>
+      <c r="D115" s="3"/>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>

</xml_diff>